<commit_message>
add func to handle text input
</commit_message>
<xml_diff>
--- a/selected_result/1_med_1000epoch_all_f1.xlsx
+++ b/selected_result/1_med_1000epoch_all_f1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taliah\code\ml_class\tcm-project\ml-tcm-nn\ML_TCM_NN\selected_result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95D9651-73C3-4F32-B879-C560B27E627B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7D6F80-25F2-4FE2-BE6D-F9FB8E941B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{EC802F3C-1A1C-420D-AC1E-837DE8976946}"/>
   </bookViews>
@@ -456,6 +456,1665 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW"/>
+              <a:t>count of 1 of the medicine</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW"/>
+              <a:t>in data set vs f1 score</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-HK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>all_f1_score_2!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>count of 1 in data</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>all_f1_score_2!$C$2:$C$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="103"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7862595419847328</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75294117647058822</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54166666666666663</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.46616541353383456</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.43478260869565216</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3728813559322034</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.37254901960784315</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.32353934481594054</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.30188679245283018</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.23684210526315788</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.22222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.17391304347826086</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.15384615384615385</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.11764705882352941</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.11764705882352941</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.10810810810810811</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.0909090909090912E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.6956521739130432E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.7142857142857141E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>all_f1_score_2!$F$2:$F$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="103"/>
+                <c:pt idx="0">
+                  <c:v>368</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>326</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-567A-4909-8636-6C222A180E01}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="783592992"/>
+        <c:axId val="664296880"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="783592992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>f1-score</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-HK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-HK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="664296880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="664296880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>count</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" baseline="0"/>
+                  <a:t> of 1</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-HK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-HK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="783592992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-HK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1636373</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>116012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4570929</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76628</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="圖表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE5AD94D-EF00-5766-33BF-645FA45449C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -794,8 +2453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D7DE39-4B9E-41C4-8FC0-7F5A71255D51}">
   <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B58" sqref="A58:XFD58"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3201,8 +4860,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>